<commit_message>
added Rectangle detection for non table data
</commit_message>
<xml_diff>
--- a/src/main/resources/static/example.xlsx
+++ b/src/main/resources/static/example.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61BA51FB-C5B3-48B9-B6F9-03D243636B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{16F5F845-029A-4FD5-B0D2-E62E8C4A5AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -514,542 +514,542 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A74EF31-A911-4131-9FED-A806CF7BE6B9}">
-  <dimension ref="L15:AF33"/>
+  <dimension ref="M22:AG40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I16" workbookViewId="0">
-      <selection activeCell="AB28" sqref="AB28:AF33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22:AG40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="15" spans="15:22">
-      <c r="O15" s="1" t="s">
+    <row r="22" spans="13:29">
+      <c r="P22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="Q22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="R22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="R15" s="1" t="s">
+      <c r="S22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S15" s="1" t="s">
+      <c r="T22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="T15" s="1" t="s">
+      <c r="U22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="U15" s="1" t="s">
+      <c r="V22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="V15" s="1" t="s">
+      <c r="W22" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="15:22">
-      <c r="O16" s="2">
+    <row r="23" spans="13:29">
+      <c r="P23" s="2">
         <v>6892</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="Q23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="R23" s="2">
         <v>28</v>
       </c>
-      <c r="R16" s="2">
+      <c r="S23" s="2">
         <v>65222</v>
       </c>
-      <c r="S16" s="2" t="s">
+      <c r="T23" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="12:32">
-      <c r="O17" s="3">
+    <row r="24" spans="13:29">
+      <c r="P24" s="3">
         <v>4561</v>
       </c>
-      <c r="P17" s="3" t="s">
+      <c r="Q24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Q17" s="3">
+      <c r="R24" s="3">
         <v>27</v>
       </c>
-      <c r="R17" s="3">
+      <c r="S24" s="3">
         <v>93335</v>
       </c>
-      <c r="S17" s="3" t="s">
+      <c r="T24" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="12:32">
-      <c r="O18" s="3">
+    <row r="25" spans="13:29">
+      <c r="P25" s="3">
         <v>7184</v>
       </c>
-      <c r="P18" s="3" t="s">
+      <c r="Q25" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Q18" s="3">
+      <c r="R25" s="3">
         <v>31</v>
       </c>
-      <c r="R18" s="3">
+      <c r="S25" s="3">
         <v>40965</v>
       </c>
-      <c r="S18" s="3" t="s">
+      <c r="T25" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="T18" s="3">
+      <c r="U25" s="3">
         <v>4561</v>
       </c>
-      <c r="U18" s="3" t="s">
+      <c r="V25" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="V18" s="3">
+      <c r="W25" s="3">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="12:32">
-      <c r="O19" s="3">
+    <row r="26" spans="13:29">
+      <c r="P26" s="3">
         <v>4099</v>
       </c>
-      <c r="P19" s="3" t="s">
+      <c r="Q26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Q19" s="3">
+      <c r="R26" s="3">
         <v>53</v>
       </c>
-      <c r="R19" s="3">
+      <c r="S26" s="3">
         <v>54538</v>
       </c>
-      <c r="S19" s="3" t="s">
+      <c r="T26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3">
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="12:32">
-      <c r="O20" s="3">
+    <row r="27" spans="13:29">
+      <c r="P27" s="3">
         <v>7278</v>
       </c>
-      <c r="P20" s="3" t="s">
+      <c r="Q27" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Q20" s="3">
+      <c r="R27" s="3">
         <v>52</v>
       </c>
-      <c r="R20" s="3">
+      <c r="S27" s="3">
         <v>38110</v>
       </c>
-      <c r="S20" s="3" t="s">
+      <c r="T27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3">
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="12:32">
-      <c r="L21" s="1" t="s">
+    <row r="28" spans="13:29">
+      <c r="M28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="N28" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="O28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O21" s="1" t="s">
+      <c r="P28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="Q28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="S21" s="1" t="s">
+      <c r="T28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T21" s="1" t="s">
+      <c r="U28" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="U21" s="1" t="s">
+      <c r="V28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="V21" s="1" t="s">
+      <c r="W28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="W21" s="1" t="s">
+      <c r="X28" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="12:32">
-      <c r="L22" s="2">
+    <row r="29" spans="13:29">
+      <c r="M29" s="2">
         <v>6892</v>
       </c>
-      <c r="M22" s="2" t="s">
+      <c r="N29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N22" s="2">
+      <c r="O29" s="2">
         <v>28</v>
       </c>
-      <c r="O22" s="2">
+      <c r="P29" s="2">
         <v>65222</v>
       </c>
-      <c r="P22" s="2" t="s">
+      <c r="Q29" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="S22" s="2">
+      <c r="T29" s="2">
         <v>6892</v>
       </c>
-      <c r="T22" s="2" t="s">
+      <c r="U29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="U22" s="2">
+      <c r="V29" s="2">
         <v>28</v>
       </c>
-      <c r="V22" s="2">
+      <c r="W29" s="2">
         <v>65222</v>
       </c>
-      <c r="W22" s="2" t="s">
+      <c r="X29" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="X22" s="1" t="s">
+      <c r="Y29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Y22" s="1" t="s">
+      <c r="Z29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z22" s="1" t="s">
+      <c r="AA29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AA22" s="1" t="s">
+      <c r="AB29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AB22" s="1" t="s">
+      <c r="AC29" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="12:32">
-      <c r="L23" s="3">
+    <row r="30" spans="13:29">
+      <c r="M30" s="3">
         <v>4561</v>
       </c>
-      <c r="M23" s="3" t="s">
+      <c r="N30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N23" s="3">
+      <c r="O30" s="3">
         <v>27</v>
       </c>
-      <c r="O23" s="3">
+      <c r="P30" s="3">
         <v>93335</v>
       </c>
-      <c r="P23" s="3" t="s">
+      <c r="Q30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="S23" s="3">
+      <c r="T30" s="3">
         <v>4561</v>
       </c>
-      <c r="T23" s="3" t="s">
+      <c r="U30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="U23" s="3">
+      <c r="V30" s="3">
         <v>27</v>
       </c>
-      <c r="V23" s="3">
+      <c r="W30" s="3">
         <v>93335</v>
       </c>
-      <c r="W23" s="3" t="s">
+      <c r="X30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="X23" s="2">
+      <c r="Y30" s="2">
         <v>6892</v>
       </c>
-      <c r="Y23" s="2" t="s">
+      <c r="Z30" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Z23" s="2">
+      <c r="AA30" s="2">
         <v>28</v>
       </c>
-      <c r="AA23" s="2">
+      <c r="AB30" s="2">
         <v>65222</v>
       </c>
-      <c r="AB23" s="2" t="s">
+      <c r="AC30" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="12:32">
-      <c r="L24" s="3">
+    <row r="31" spans="13:29">
+      <c r="M31" s="3">
         <v>7184</v>
       </c>
-      <c r="M24" s="3" t="s">
+      <c r="N31" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N24" s="3">
+      <c r="O31" s="3">
         <v>31</v>
       </c>
-      <c r="O24" s="3">
+      <c r="P31" s="3">
         <v>40965</v>
       </c>
-      <c r="P24" s="3" t="s">
+      <c r="Q31" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="S24" s="3">
+      <c r="T31" s="3">
         <v>7184</v>
       </c>
-      <c r="T24" s="3" t="s">
+      <c r="U31" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="U24" s="3">
+      <c r="V31" s="3">
         <v>31</v>
       </c>
-      <c r="V24" s="3">
+      <c r="W31" s="3">
         <v>40965</v>
       </c>
-      <c r="W24" s="3" t="s">
+      <c r="X31" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="X24" s="3">
+      <c r="Y31" s="3">
         <v>4561</v>
       </c>
-      <c r="Y24" s="3" t="s">
+      <c r="Z31" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Z24" s="3">
+      <c r="AA31" s="3">
         <v>27</v>
       </c>
-      <c r="AA24" s="3">
+      <c r="AB31" s="3">
         <v>93335</v>
       </c>
-      <c r="AB24" s="3" t="s">
+      <c r="AC31" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="12:32">
-      <c r="L25" s="3">
+    <row r="32" spans="13:29">
+      <c r="M32" s="3">
         <v>4099</v>
       </c>
-      <c r="M25" s="3" t="s">
+      <c r="N32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N25" s="3">
+      <c r="O32" s="3">
         <v>53</v>
       </c>
-      <c r="O25" s="3">
+      <c r="P32" s="3">
         <v>54538</v>
       </c>
-      <c r="P25" s="3" t="s">
+      <c r="Q32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="S25" s="3">
+      <c r="T32" s="3">
         <v>4099</v>
       </c>
-      <c r="T25" s="3" t="s">
+      <c r="U32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="U25" s="3">
+      <c r="V32" s="3">
         <v>53</v>
       </c>
-      <c r="V25" s="3">
+      <c r="W32" s="3">
         <v>54538</v>
       </c>
-      <c r="W25" s="3" t="s">
+      <c r="X32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="X25" s="3">
+      <c r="Y32" s="3">
         <v>7184</v>
       </c>
-      <c r="Y25" s="3" t="s">
+      <c r="Z32" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Z25" s="3">
+      <c r="AA32" s="3">
         <v>31</v>
       </c>
-      <c r="AA25" s="3">
+      <c r="AB32" s="3">
         <v>40965</v>
       </c>
-      <c r="AB25" s="3" t="s">
+      <c r="AC32" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="12:32">
-      <c r="L26" s="3">
+    <row r="33" spans="13:33">
+      <c r="M33" s="3">
         <v>7278</v>
       </c>
-      <c r="M26" s="3" t="s">
+      <c r="N33" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N26" s="3">
+      <c r="O33" s="3">
         <v>52</v>
       </c>
-      <c r="O26" s="3">
+      <c r="P33" s="3">
         <v>38110</v>
       </c>
-      <c r="P26" s="3" t="s">
+      <c r="Q33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="S26" s="3">
+      <c r="T33" s="3">
         <v>7278</v>
       </c>
-      <c r="T26" s="3" t="s">
+      <c r="U33" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="U26" s="3">
+      <c r="V33" s="3">
         <v>52</v>
       </c>
-      <c r="V26" s="3">
+      <c r="W33" s="3">
         <v>38110</v>
       </c>
-      <c r="W26" s="3" t="s">
+      <c r="X33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="X26" s="3">
+      <c r="Y33" s="3">
         <v>4099</v>
       </c>
-      <c r="Y26" s="3" t="s">
+      <c r="Z33" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Z26" s="3">
+      <c r="AA33" s="3">
         <v>53</v>
       </c>
-      <c r="AA26" s="3">
+      <c r="AB33" s="3">
         <v>54538</v>
       </c>
-      <c r="AB26" s="3" t="s">
+      <c r="AC33" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="12:32">
-      <c r="X27" s="3">
+    <row r="34" spans="13:33">
+      <c r="Y34" s="3">
         <v>7278</v>
       </c>
-      <c r="Y27" s="3" t="s">
+      <c r="Z34" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Z27" s="3">
+      <c r="AA34" s="3">
         <v>52</v>
       </c>
-      <c r="AA27" s="3">
+      <c r="AB34" s="3">
         <v>38110</v>
       </c>
-      <c r="AB27" s="3" t="s">
+      <c r="AC34" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="12:32">
-      <c r="L28" s="3">
+    <row r="35" spans="13:33">
+      <c r="M35" s="3">
         <v>7278</v>
       </c>
-      <c r="M28" s="3" t="s">
+      <c r="N35" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N28" s="3">
+      <c r="O35" s="3">
         <v>52</v>
       </c>
-      <c r="O28" s="3">
+      <c r="P35" s="3">
         <v>38110</v>
       </c>
-      <c r="P28" s="3" t="s">
+      <c r="Q35" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AB28" s="1" t="s">
+      <c r="AC35" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AC28" s="1" t="s">
+      <c r="AD35" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AD28" s="1" t="s">
+      <c r="AE35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AE28" s="1" t="s">
+      <c r="AF35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AF28" s="1" t="s">
+      <c r="AG35" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="12:32">
-      <c r="AB29" s="2">
+    <row r="36" spans="13:33">
+      <c r="AC36" s="2">
         <v>6892</v>
       </c>
-      <c r="AC29" s="2" t="s">
+      <c r="AD36" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AD29" s="2">
+      <c r="AE36" s="2">
         <v>28</v>
       </c>
-      <c r="AE29" s="2">
+      <c r="AF36" s="2">
         <v>65222</v>
       </c>
-      <c r="AF29" s="2" t="s">
+      <c r="AG36" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="12:32">
-      <c r="AB30" s="3">
+    <row r="37" spans="13:33">
+      <c r="AC37" s="3">
         <v>4561</v>
       </c>
-      <c r="AC30" s="3" t="s">
+      <c r="AD37" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AD30" s="3">
+      <c r="AE37" s="3">
         <v>27</v>
       </c>
-      <c r="AE30" s="3">
+      <c r="AF37" s="3">
         <v>93335</v>
       </c>
-      <c r="AF30" s="3" t="s">
+      <c r="AG37" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="12:32">
-      <c r="AB31" s="3">
+    <row r="38" spans="13:33">
+      <c r="AC38" s="3">
         <v>7184</v>
       </c>
-      <c r="AC31" s="3" t="s">
+      <c r="AD38" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AD31" s="3">
+      <c r="AE38" s="3">
         <v>31</v>
       </c>
-      <c r="AE31" s="3">
+      <c r="AF38" s="3">
         <v>40965</v>
       </c>
-      <c r="AF31" s="3" t="s">
+      <c r="AG38" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="12:32">
-      <c r="AB32" s="3">
+    <row r="39" spans="13:33">
+      <c r="AC39" s="3">
         <v>4099</v>
       </c>
-      <c r="AC32" s="3" t="s">
+      <c r="AD39" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AD32" s="3">
+      <c r="AE39" s="3">
         <v>53</v>
       </c>
-      <c r="AE32" s="3">
+      <c r="AF39" s="3">
         <v>54538</v>
       </c>
-      <c r="AF32" s="3" t="s">
+      <c r="AG39" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="28:32">
-      <c r="AB33" s="3">
+    <row r="40" spans="13:33">
+      <c r="AC40" s="3">
         <v>7278</v>
       </c>
-      <c r="AC33" s="3" t="s">
+      <c r="AD40" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AD33" s="3">
+      <c r="AE40" s="3">
         <v>52</v>
       </c>
-      <c r="AE33" s="3">
+      <c r="AF40" s="3">
         <v>38110</v>
       </c>
-      <c r="AF33" s="3" t="s">
+      <c r="AG40" s="3" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>